<commit_message>
update: files, readme, core
</commit_message>
<xml_diff>
--- a/output/output_vietocr.xlsx
+++ b/output/output_vietocr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,9 +433,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="32" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,170 +452,187 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Khu vực</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>Ký hiệu chữ viết tắt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>Chữ viết đây đủ</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Toàn thế giới</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4,1</t>
+          <t>TDTT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2,7</t>
+          <t>Thể dục thể thao</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Các nước phát triển</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3,0</t>
+          <t>HĐND</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1,6</t>
+          <t>Hội đông nhân dân</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Các nước đang phát triển:</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7,3</t>
+          <t>UBND</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6,0</t>
+          <t>ủy ban nhân dân</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Đông Á và thái bình dương</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9,7</t>
+          <t>KH</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8,2</t>
+          <t>Kế hoạch</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>- Đông Âu và trung Á</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5,2</t>
+          <t>ATGT QL 217</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5,3</t>
+          <t>An toàn giao thông Quốc lộ 217</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>- Châu Mỹ Latinh và Caribe</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6,0</t>
+          <t>UBDS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4,2</t>
+          <t>Ủy ban dân số</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>- Trung Đông và bắc phi</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3,6</t>
+          <t>THPT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1,7</t>
+          <t>Trung học phố thông</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>- Nam Á 1990.000000099000</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9,1</t>
+          <t>TE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6,6</t>
+          <t>Trẻ em</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>- Cận Sahara châu phi</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>CĐ-ĐH</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>Cao đẳng - đại học</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CNH- HĐH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Công nghiệp hóa- hiện đại hóa</t>
         </is>
       </c>
     </row>

</xml_diff>